<commit_message>
run all inputs except financial flows
</commit_message>
<xml_diff>
--- a/concepts/deforestation/input.xlsx
+++ b/concepts/deforestation/input.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="89">
   <si>
     <t>Pattern name (optional)</t>
   </si>
@@ -75,130 +75,136 @@
     <t>forest</t>
   </si>
   <si>
+    <t>Tropical forests</t>
+  </si>
+  <si>
+    <t>Tropical forest</t>
+  </si>
+  <si>
+    <t>LOWER</t>
+  </si>
+  <si>
+    <t>tropical</t>
+  </si>
+  <si>
+    <t>Rainforests</t>
+  </si>
+  <si>
+    <t>rainforest</t>
+  </si>
+  <si>
     <t>deforestation</t>
   </si>
   <si>
-    <t>LOWER</t>
-  </si>
-  <si>
-    <t>tropical deforestation</t>
-  </si>
-  <si>
-    <t>tropical</t>
+    <t>Reforestation</t>
+  </si>
+  <si>
+    <t>reforestation</t>
+  </si>
+  <si>
+    <t>reforest</t>
+  </si>
+  <si>
+    <t>Aforestation</t>
+  </si>
+  <si>
+    <t>aforestation</t>
+  </si>
+  <si>
+    <t>aforest</t>
+  </si>
+  <si>
+    <t>Illegal logging</t>
+  </si>
+  <si>
+    <t>illegal</t>
+  </si>
+  <si>
+    <t>logging</t>
+  </si>
+  <si>
+    <t>Forest-risk commodities</t>
+  </si>
+  <si>
+    <t>forest-risk commodities</t>
+  </si>
+  <si>
+    <t>ORTH</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>OP</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>risk</t>
+  </si>
+  <si>
+    <t>commodity</t>
+  </si>
+  <si>
+    <t>palm</t>
+  </si>
+  <si>
+    <t>oil</t>
+  </si>
+  <si>
+    <t>soy</t>
+  </si>
+  <si>
+    <t>soya</t>
+  </si>
+  <si>
+    <t>soybean</t>
+  </si>
+  <si>
+    <t>cereal</t>
+  </si>
+  <si>
+    <t>maize</t>
+  </si>
+  <si>
+    <t>cattle</t>
+  </si>
+  <si>
+    <t>cocoa</t>
+  </si>
+  <si>
+    <t>timber</t>
+  </si>
+  <si>
+    <t>coffee</t>
+  </si>
+  <si>
+    <t>rubber</t>
+  </si>
+  <si>
+    <t>pulp</t>
+  </si>
+  <si>
+    <t>beef</t>
+  </si>
+  <si>
+    <t>leather</t>
+  </si>
+  <si>
+    <t>corn</t>
+  </si>
+  <si>
+    <t>paper</t>
   </si>
   <si>
     <t>LEMMA_IN</t>
   </si>
   <si>
-    <t>in,of</t>
-  </si>
-  <si>
-    <t>the</t>
-  </si>
-  <si>
-    <t>Amazon</t>
-  </si>
-  <si>
-    <t>Congo,Congolian</t>
-  </si>
-  <si>
-    <t>tropical forest degradation</t>
-  </si>
-  <si>
-    <t>degradation</t>
-  </si>
-  <si>
-    <t>of</t>
-  </si>
-  <si>
-    <t>forest,rainforest</t>
-  </si>
-  <si>
-    <t>of,in</t>
-  </si>
-  <si>
-    <t>reforestation</t>
-  </si>
-  <si>
-    <t>reforest</t>
-  </si>
-  <si>
-    <t>aforestation</t>
-  </si>
-  <si>
-    <t>aforest</t>
-  </si>
-  <si>
-    <t>forest-risk commodities</t>
-  </si>
-  <si>
-    <t>ORTH</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>OP</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>risk</t>
-  </si>
-  <si>
-    <t>commodity</t>
-  </si>
-  <si>
-    <t>palm</t>
-  </si>
-  <si>
-    <t>oil</t>
-  </si>
-  <si>
-    <t>soy</t>
-  </si>
-  <si>
-    <t>soya</t>
-  </si>
-  <si>
-    <t>soybean</t>
-  </si>
-  <si>
-    <t>cereal</t>
-  </si>
-  <si>
-    <t>maize</t>
-  </si>
-  <si>
-    <t>cattle</t>
-  </si>
-  <si>
-    <t>cocoa</t>
-  </si>
-  <si>
-    <t>timber</t>
-  </si>
-  <si>
-    <t>coffee</t>
-  </si>
-  <si>
-    <t>rubber</t>
-  </si>
-  <si>
-    <t>paper</t>
-  </si>
-  <si>
-    <t>pulp</t>
-  </si>
-  <si>
-    <t>beef</t>
-  </si>
-  <si>
-    <t>leather</t>
-  </si>
-  <si>
-    <t>corn</t>
+    <t>industry,manufacturing</t>
+  </si>
+  <si>
+    <t>make,manufacture</t>
   </si>
   <si>
     <r>
@@ -377,18 +383,13 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border/>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -433,12 +434,6 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
@@ -871,22 +866,24 @@
       <c r="B4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>20</v>
-      </c>
+      <c r="C4" s="9"/>
       <c r="D4" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="12" t="s">
         <v>21</v>
       </c>
+      <c r="E4" s="10" t="s">
+        <v>22</v>
+      </c>
       <c r="F4" s="10" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
+      <c r="I4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="K4" s="11"/>
       <c r="L4" s="11"/>
       <c r="M4" s="11"/>
@@ -913,38 +910,34 @@
       <c r="AJ4" s="11"/>
     </row>
     <row r="5">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>23</v>
+      <c r="A5" s="14"/>
+      <c r="B5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
-      <c r="I5" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>20</v>
-      </c>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
       <c r="K5" s="11"/>
-      <c r="L5" s="17"/>
+      <c r="L5" s="11"/>
       <c r="M5" s="11"/>
       <c r="N5" s="11"/>
       <c r="O5" s="11"/>
-      <c r="P5" s="17"/>
+      <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
       <c r="R5" s="11"/>
       <c r="S5" s="11"/>
-      <c r="T5" s="17"/>
+      <c r="T5" s="11"/>
       <c r="U5" s="13"/>
       <c r="W5" s="13"/>
       <c r="Y5" s="11"/>
@@ -961,46 +954,36 @@
       <c r="AJ5" s="11"/>
     </row>
     <row r="6">
-      <c r="A6" s="15"/>
-      <c r="B6" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="16" t="s">
-        <v>22</v>
+      <c r="A6" s="14"/>
+      <c r="B6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>26</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
-      <c r="I6" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>25</v>
-      </c>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
       <c r="K6" s="11"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="N6" s="11" t="s">
-        <v>26</v>
-      </c>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
       <c r="O6" s="11"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="R6" s="11" t="s">
-        <v>27</v>
-      </c>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
       <c r="S6" s="11"/>
-      <c r="T6" s="17"/>
+      <c r="T6" s="11"/>
       <c r="U6" s="13"/>
       <c r="W6" s="13"/>
       <c r="Y6" s="11"/>
@@ -1018,45 +1001,34 @@
     </row>
     <row r="7">
       <c r="A7" s="15"/>
-      <c r="B7" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>20</v>
+      <c r="B7" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>29</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
-      <c r="I7" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>25</v>
-      </c>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
       <c r="K7" s="11"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="N7" s="11" t="s">
-        <v>26</v>
-      </c>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
       <c r="O7" s="11"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="R7" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="S7" s="11"/>
-      <c r="T7" s="17"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="13"/>
       <c r="U7" s="13"/>
       <c r="W7" s="13"/>
       <c r="Y7" s="11"/>
@@ -1074,41 +1046,34 @@
     </row>
     <row r="8">
       <c r="A8" s="15"/>
-      <c r="B8" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>20</v>
+      <c r="B8" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
-      <c r="I8" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>25</v>
-      </c>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
       <c r="K8" s="11"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="N8" s="11" t="s">
-        <v>28</v>
-      </c>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
       <c r="O8" s="11"/>
-      <c r="P8" s="17"/>
+      <c r="P8" s="11"/>
       <c r="Q8" s="11"/>
       <c r="R8" s="11"/>
-      <c r="S8" s="11"/>
-      <c r="T8" s="17"/>
+      <c r="S8" s="13"/>
       <c r="U8" s="13"/>
       <c r="W8" s="13"/>
       <c r="Y8" s="11"/>
@@ -1127,40 +1092,35 @@
     <row r="9">
       <c r="A9" s="15"/>
       <c r="B9" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>23</v>
+        <v>33</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
-      <c r="I9" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>19</v>
+      <c r="I9" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="K9" s="11"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="N9" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="O9" s="11"/>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="11"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="17"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="13"/>
       <c r="U9" s="13"/>
       <c r="W9" s="13"/>
       <c r="Y9" s="11"/>
@@ -1179,44 +1139,49 @@
     <row r="10">
       <c r="A10" s="15"/>
       <c r="B10" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18" t="s">
-        <v>29</v>
+        <v>36</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>30</v>
+        <v>22</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>19</v>
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
-      <c r="I10" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J10" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="K10" s="11"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="N10" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="O10" s="11"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="R10" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="S10" s="11"/>
-      <c r="T10" s="17"/>
+      <c r="I10" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="R10" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="S10" s="13"/>
       <c r="U10" s="13"/>
       <c r="W10" s="13"/>
       <c r="Y10" s="11"/>
@@ -1235,42 +1200,35 @@
     <row r="11">
       <c r="A11" s="15"/>
       <c r="B11" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18" t="s">
-        <v>29</v>
+        <v>36</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>30</v>
+        <v>22</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
-      <c r="I11" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="J11" s="11" t="s">
-        <v>33</v>
+      <c r="I11" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="K11" s="11"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="N11" s="11" t="s">
-        <v>26</v>
-      </c>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
       <c r="O11" s="11"/>
-      <c r="P11" s="17"/>
+      <c r="P11" s="11"/>
       <c r="Q11" s="11"/>
-      <c r="R11" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="S11" s="11"/>
-      <c r="T11" s="17"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="13"/>
       <c r="U11" s="13"/>
       <c r="W11" s="13"/>
       <c r="Y11" s="11"/>
@@ -1289,42 +1247,25 @@
     <row r="12">
       <c r="A12" s="15"/>
       <c r="B12" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="J12" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="K12" s="11"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="N12" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="O12" s="11"/>
-      <c r="P12" s="17"/>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="S12" s="11"/>
-      <c r="T12" s="17"/>
+        <v>36</v>
+      </c>
+      <c r="C12" s="17"/>
+      <c r="D12" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="13"/>
+      <c r="I12" s="11"/>
+      <c r="K12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="Q12" s="13"/>
+      <c r="S12" s="13"/>
       <c r="U12" s="13"/>
       <c r="W12" s="13"/>
       <c r="Y12" s="11"/>
@@ -1343,40 +1284,25 @@
     <row r="13">
       <c r="A13" s="15"/>
       <c r="B13" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16" t="s">
-        <v>29</v>
+        <v>36</v>
+      </c>
+      <c r="C13" s="17"/>
+      <c r="D13" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="K13" s="11"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="N13" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="O13" s="11"/>
-      <c r="P13" s="17"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="11"/>
-      <c r="S13" s="11"/>
-      <c r="T13" s="17"/>
+        <v>22</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="13"/>
+      <c r="I13" s="12"/>
+      <c r="K13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="Q13" s="13"/>
+      <c r="S13" s="13"/>
       <c r="U13" s="13"/>
       <c r="W13" s="13"/>
       <c r="Y13" s="11"/>
@@ -1395,32 +1321,24 @@
     <row r="14">
       <c r="A14" s="15"/>
       <c r="B14" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>34</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C14" s="17"/>
       <c r="D14" s="9" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E14" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
+      <c r="F14" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" s="13"/>
       <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="11"/>
-      <c r="O14" s="11"/>
-      <c r="P14" s="11"/>
-      <c r="Q14" s="11"/>
-      <c r="R14" s="11"/>
+      <c r="K14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="Q14" s="13"/>
       <c r="S14" s="13"/>
       <c r="U14" s="13"/>
       <c r="W14" s="13"/>
@@ -1442,30 +1360,22 @@
       <c r="B15" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>36</v>
-      </c>
+      <c r="C15" s="17"/>
       <c r="D15" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E15" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="11"/>
+      <c r="F15" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="Q15" s="13"/>
       <c r="S15" s="13"/>
       <c r="U15" s="13"/>
       <c r="W15" s="13"/>
@@ -1485,48 +1395,24 @@
     <row r="16">
       <c r="A16" s="15"/>
       <c r="B16" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>38</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C16" s="17"/>
       <c r="D16" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="J16" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="K16" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="L16" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="M16" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="N16" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="O16" s="12"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="R16" s="10" t="s">
-        <v>44</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="Q16" s="13"/>
       <c r="S16" s="13"/>
       <c r="U16" s="13"/>
       <c r="W16" s="13"/>
@@ -1546,34 +1432,24 @@
     <row r="17">
       <c r="A17" s="15"/>
       <c r="B17" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="16"/>
+        <v>36</v>
+      </c>
+      <c r="C17" s="17"/>
       <c r="D17" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J17" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="11"/>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="11"/>
-      <c r="R17" s="11"/>
+        <v>37</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="Q17" s="13"/>
       <c r="S17" s="13"/>
       <c r="U17" s="13"/>
       <c r="W17" s="13"/>
@@ -1593,20 +1469,20 @@
     <row r="18">
       <c r="A18" s="15"/>
       <c r="B18" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="19"/>
+        <v>36</v>
+      </c>
+      <c r="C18" s="17"/>
       <c r="D18" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>47</v>
+        <v>37</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>52</v>
       </c>
       <c r="G18" s="13"/>
-      <c r="I18" s="11"/>
+      <c r="I18" s="13"/>
       <c r="K18" s="13"/>
       <c r="M18" s="13"/>
       <c r="O18" s="13"/>
@@ -1630,20 +1506,20 @@
     <row r="19">
       <c r="A19" s="15"/>
       <c r="B19" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="19"/>
+        <v>36</v>
+      </c>
+      <c r="C19" s="17"/>
       <c r="D19" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>48</v>
+        <v>37</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>53</v>
       </c>
       <c r="G19" s="13"/>
-      <c r="I19" s="12"/>
+      <c r="I19" s="13"/>
       <c r="K19" s="13"/>
       <c r="M19" s="13"/>
       <c r="O19" s="13"/>
@@ -1667,20 +1543,20 @@
     <row r="20">
       <c r="A20" s="15"/>
       <c r="B20" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="19"/>
+        <v>36</v>
+      </c>
+      <c r="C20" s="17"/>
       <c r="D20" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" s="20" t="s">
-        <v>49</v>
+        <v>22</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>54</v>
       </c>
       <c r="G20" s="13"/>
-      <c r="I20" s="12"/>
+      <c r="I20" s="13"/>
       <c r="K20" s="13"/>
       <c r="M20" s="13"/>
       <c r="O20" s="13"/>
@@ -1704,17 +1580,17 @@
     <row r="21">
       <c r="A21" s="15"/>
       <c r="B21" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="19"/>
+        <v>36</v>
+      </c>
+      <c r="C21" s="17"/>
       <c r="D21" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21" s="20" t="s">
-        <v>50</v>
+        <v>22</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>55</v>
       </c>
       <c r="G21" s="13"/>
       <c r="I21" s="13"/>
@@ -1741,17 +1617,17 @@
     <row r="22">
       <c r="A22" s="15"/>
       <c r="B22" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" s="19"/>
+        <v>36</v>
+      </c>
+      <c r="C22" s="17"/>
       <c r="D22" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>51</v>
+        <v>22</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>56</v>
       </c>
       <c r="G22" s="13"/>
       <c r="I22" s="13"/>
@@ -1778,17 +1654,17 @@
     <row r="23">
       <c r="A23" s="15"/>
       <c r="B23" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="19"/>
+        <v>36</v>
+      </c>
+      <c r="C23" s="17"/>
       <c r="D23" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F23" s="20" t="s">
-        <v>52</v>
+        <v>22</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>57</v>
       </c>
       <c r="G23" s="13"/>
       <c r="I23" s="13"/>
@@ -1815,17 +1691,17 @@
     <row r="24">
       <c r="A24" s="15"/>
       <c r="B24" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" s="19"/>
+        <v>36</v>
+      </c>
+      <c r="C24" s="17"/>
       <c r="D24" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F24" s="20" t="s">
-        <v>53</v>
+        <v>22</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>58</v>
       </c>
       <c r="G24" s="13"/>
       <c r="I24" s="13"/>
@@ -1852,17 +1728,17 @@
     <row r="25">
       <c r="A25" s="15"/>
       <c r="B25" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="19"/>
+        <v>36</v>
+      </c>
+      <c r="C25" s="17"/>
       <c r="D25" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F25" s="20" t="s">
-        <v>54</v>
+        <v>22</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>59</v>
       </c>
       <c r="G25" s="13"/>
       <c r="I25" s="13"/>
@@ -1889,20 +1765,25 @@
     <row r="26">
       <c r="A26" s="15"/>
       <c r="B26" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C26" s="19"/>
+        <v>36</v>
+      </c>
+      <c r="C26" s="17"/>
       <c r="D26" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F26" s="20" t="s">
-        <v>55</v>
+        <v>22</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>60</v>
       </c>
       <c r="G26" s="13"/>
-      <c r="I26" s="13"/>
+      <c r="I26" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="J26" s="18" t="s">
+        <v>62</v>
+      </c>
       <c r="K26" s="13"/>
       <c r="M26" s="13"/>
       <c r="O26" s="13"/>
@@ -1926,20 +1807,25 @@
     <row r="27">
       <c r="A27" s="15"/>
       <c r="B27" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="19"/>
+        <v>36</v>
+      </c>
+      <c r="C27" s="17"/>
       <c r="D27" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F27" s="20" t="s">
-        <v>56</v>
+        <v>37</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>63</v>
       </c>
       <c r="G27" s="13"/>
-      <c r="I27" s="13"/>
+      <c r="I27" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J27" s="18" t="s">
+        <v>60</v>
+      </c>
       <c r="K27" s="13"/>
       <c r="M27" s="13"/>
       <c r="O27" s="13"/>
@@ -1960,191 +1846,6 @@
       <c r="AI27" s="11"/>
       <c r="AJ27" s="11"/>
     </row>
-    <row r="28">
-      <c r="A28" s="15"/>
-      <c r="B28" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C28" s="19"/>
-      <c r="D28" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F28" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="G28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="O28" s="13"/>
-      <c r="Q28" s="13"/>
-      <c r="S28" s="13"/>
-      <c r="U28" s="13"/>
-      <c r="W28" s="13"/>
-      <c r="Y28" s="11"/>
-      <c r="Z28" s="11"/>
-      <c r="AA28" s="11"/>
-      <c r="AB28" s="11"/>
-      <c r="AC28" s="11"/>
-      <c r="AD28" s="11"/>
-      <c r="AE28" s="11"/>
-      <c r="AF28" s="11"/>
-      <c r="AG28" s="11"/>
-      <c r="AH28" s="11"/>
-      <c r="AI28" s="11"/>
-      <c r="AJ28" s="11"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="15"/>
-      <c r="B29" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C29" s="19"/>
-      <c r="D29" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F29" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="G29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="K29" s="13"/>
-      <c r="M29" s="13"/>
-      <c r="O29" s="13"/>
-      <c r="Q29" s="13"/>
-      <c r="S29" s="13"/>
-      <c r="U29" s="13"/>
-      <c r="W29" s="13"/>
-      <c r="Y29" s="11"/>
-      <c r="Z29" s="11"/>
-      <c r="AA29" s="11"/>
-      <c r="AB29" s="11"/>
-      <c r="AC29" s="11"/>
-      <c r="AD29" s="11"/>
-      <c r="AE29" s="11"/>
-      <c r="AF29" s="11"/>
-      <c r="AG29" s="11"/>
-      <c r="AH29" s="11"/>
-      <c r="AI29" s="11"/>
-      <c r="AJ29" s="11"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="15"/>
-      <c r="B30" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C30" s="19"/>
-      <c r="D30" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F30" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="G30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="K30" s="13"/>
-      <c r="M30" s="13"/>
-      <c r="O30" s="13"/>
-      <c r="Q30" s="13"/>
-      <c r="S30" s="13"/>
-      <c r="U30" s="13"/>
-      <c r="W30" s="13"/>
-      <c r="Y30" s="11"/>
-      <c r="Z30" s="11"/>
-      <c r="AA30" s="11"/>
-      <c r="AB30" s="11"/>
-      <c r="AC30" s="11"/>
-      <c r="AD30" s="11"/>
-      <c r="AE30" s="11"/>
-      <c r="AF30" s="11"/>
-      <c r="AG30" s="11"/>
-      <c r="AH30" s="11"/>
-      <c r="AI30" s="11"/>
-      <c r="AJ30" s="11"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="15"/>
-      <c r="B31" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F31" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="G31" s="13"/>
-      <c r="I31" s="13"/>
-      <c r="K31" s="13"/>
-      <c r="M31" s="13"/>
-      <c r="O31" s="13"/>
-      <c r="Q31" s="13"/>
-      <c r="S31" s="13"/>
-      <c r="U31" s="13"/>
-      <c r="W31" s="13"/>
-      <c r="Y31" s="11"/>
-      <c r="Z31" s="11"/>
-      <c r="AA31" s="11"/>
-      <c r="AB31" s="11"/>
-      <c r="AC31" s="11"/>
-      <c r="AD31" s="11"/>
-      <c r="AE31" s="11"/>
-      <c r="AF31" s="11"/>
-      <c r="AG31" s="11"/>
-      <c r="AH31" s="11"/>
-      <c r="AI31" s="11"/>
-      <c r="AJ31" s="11"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="15"/>
-      <c r="B32" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C32" s="19"/>
-      <c r="D32" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F32" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="G32" s="13"/>
-      <c r="I32" s="13"/>
-      <c r="K32" s="13"/>
-      <c r="M32" s="13"/>
-      <c r="O32" s="13"/>
-      <c r="Q32" s="13"/>
-      <c r="S32" s="13"/>
-      <c r="U32" s="13"/>
-      <c r="W32" s="13"/>
-      <c r="Y32" s="11"/>
-      <c r="Z32" s="11"/>
-      <c r="AA32" s="11"/>
-      <c r="AB32" s="11"/>
-      <c r="AC32" s="11"/>
-      <c r="AD32" s="11"/>
-      <c r="AE32" s="11"/>
-      <c r="AF32" s="11"/>
-      <c r="AG32" s="11"/>
-      <c r="AH32" s="11"/>
-      <c r="AI32" s="11"/>
-      <c r="AJ32" s="11"/>
-    </row>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="Q1:T1"/>
@@ -2161,7 +1862,7 @@
     <mergeCell ref="M1:P1"/>
   </mergeCells>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3:E32 G3:G32 I3:I32 K3:K32 M3:M32 O3:O32 Q3:Q32 S3:S32 U3:U32 W3:W32 Y3:Y32 AA3:AA32 AC3:AC32 AE3:AE32 AG3:AG32 AI3:AI32">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3:E27 G3:G27 I3:I27 K3:K27 M3:M27 O3:O27 Q3:Q27 S3:S27 U3:U27 W3:W27 Y3:Y27 AA3:AA27 AC3:AC27 AE3:AE27 AG3:AG27 AI3:AI27">
       <formula1>'Rule types'!$A$3:$A$100</formula1>
     </dataValidation>
   </dataValidations>
@@ -2180,148 +1881,148 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="21" t="s">
-        <v>62</v>
+      <c r="A1" s="19" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="20" t="s">
-        <v>39</v>
+      <c r="A3" s="18" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="20" t="s">
-        <v>63</v>
+      <c r="A4" s="18" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="20" t="s">
-        <v>64</v>
+      <c r="A5" s="18" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="20" t="s">
-        <v>21</v>
+      <c r="A6" s="18" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="20" t="s">
-        <v>65</v>
+      <c r="A7" s="18" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="20" t="s">
-        <v>66</v>
+      <c r="A8" s="18" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="20" t="s">
-        <v>67</v>
+      <c r="A9" s="18" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="20" t="s">
-        <v>68</v>
+      <c r="A10" s="18" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="20" t="s">
-        <v>69</v>
+      <c r="A11" s="18" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="20" t="s">
-        <v>70</v>
+      <c r="A12" s="18" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="20" t="s">
-        <v>71</v>
+      <c r="A13" s="18" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="20" t="s">
-        <v>72</v>
+      <c r="A14" s="18" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="20" t="s">
-        <v>73</v>
+      <c r="A15" s="18" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="20" t="s">
-        <v>74</v>
+      <c r="A16" s="18" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="20" t="s">
-        <v>75</v>
+      <c r="A17" s="18" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="20" t="s">
-        <v>76</v>
+      <c r="A18" s="18" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="20" t="s">
-        <v>77</v>
+      <c r="A19" s="18" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="20" t="s">
-        <v>78</v>
+      <c r="A20" s="18" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="20" t="s">
-        <v>79</v>
+      <c r="A21" s="18" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="20" t="s">
-        <v>80</v>
+      <c r="A22" s="18" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="20" t="s">
-        <v>81</v>
+      <c r="A23" s="18" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="20" t="s">
-        <v>82</v>
+      <c r="A24" s="18" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="20" t="s">
-        <v>83</v>
+      <c r="A25" s="18" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="18" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="20" t="s">
-        <v>84</v>
+      <c r="A27" s="18" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="20" t="s">
-        <v>24</v>
+      <c r="A28" s="18" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="20" t="s">
-        <v>41</v>
+      <c r="A29" s="18" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="20" t="s">
-        <v>85</v>
+      <c r="A30" s="18" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2346,8 +2047,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="22" t="s">
-        <v>86</v>
+      <c r="A1" s="20" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
run final set of explorer inputs
</commit_message>
<xml_diff>
--- a/concepts/deforestation/input.xlsx
+++ b/concepts/deforestation/input.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="105">
   <si>
     <t>Pattern name (optional)</t>
   </si>
@@ -75,6 +75,18 @@
     <t>forest</t>
   </si>
   <si>
+    <t>Forestry</t>
+  </si>
+  <si>
+    <t>forestry</t>
+  </si>
+  <si>
+    <t>Woodlands</t>
+  </si>
+  <si>
+    <t>woodland</t>
+  </si>
+  <si>
     <t>Tropical forests</t>
   </si>
   <si>
@@ -96,6 +108,24 @@
     <t>deforestation</t>
   </si>
   <si>
+    <t>forest degradation</t>
+  </si>
+  <si>
+    <t>degradation</t>
+  </si>
+  <si>
+    <t>REDD</t>
+  </si>
+  <si>
+    <t>IS_UPPER</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>REDD+</t>
+  </si>
+  <si>
     <t>Reforestation</t>
   </si>
   <si>
@@ -105,13 +135,46 @@
     <t>reforest</t>
   </si>
   <si>
-    <t>Aforestation</t>
+    <t>Afforestation</t>
   </si>
   <si>
     <t>aforestation</t>
   </si>
   <si>
-    <t>aforest</t>
+    <t>afforestation</t>
+  </si>
+  <si>
+    <t>afforest</t>
+  </si>
+  <si>
+    <t>plant</t>
+  </si>
+  <si>
+    <t>trees</t>
+  </si>
+  <si>
+    <t>tree</t>
+  </si>
+  <si>
+    <t>ORTH</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>OP</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>planting</t>
+  </si>
+  <si>
+    <t>Revegetation</t>
+  </si>
+  <si>
+    <t>revegetation</t>
   </si>
   <si>
     <t>Illegal logging</t>
@@ -127,18 +190,6 @@
   </si>
   <si>
     <t>forest-risk commodities</t>
-  </si>
-  <si>
-    <t>ORTH</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>OP</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
   <si>
     <t>risk</t>
@@ -260,9 +311,6 @@
   </si>
   <si>
     <t>IS_LOWER</t>
-  </si>
-  <si>
-    <t>IS_UPPER</t>
   </si>
   <si>
     <t>IS_TITLE</t>
@@ -383,13 +431,18 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border/>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -434,6 +487,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
@@ -864,26 +920,22 @@
     <row r="4">
       <c r="A4" s="14"/>
       <c r="B4" s="9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>21</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>23</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
-      <c r="I4" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>19</v>
-      </c>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
       <c r="K4" s="11"/>
       <c r="L4" s="11"/>
       <c r="M4" s="11"/>
@@ -912,22 +964,22 @@
     <row r="5">
       <c r="A5" s="14"/>
       <c r="B5" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>18</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
       <c r="M5" s="11"/>
@@ -956,24 +1008,26 @@
     <row r="6">
       <c r="A6" s="14"/>
       <c r="B6" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>26</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C6" s="9"/>
       <c r="D6" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>26</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
+      <c r="I6" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
       <c r="M6" s="11"/>
@@ -1000,13 +1054,11 @@
       <c r="AJ6" s="11"/>
     </row>
     <row r="7">
-      <c r="A7" s="15"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="9" t="s">
         <v>28</v>
       </c>
+      <c r="C7" s="9"/>
       <c r="D7" s="9" t="s">
         <v>28</v>
       </c>
@@ -1028,7 +1080,8 @@
       <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
       <c r="R7" s="11"/>
-      <c r="S7" s="13"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
       <c r="U7" s="13"/>
       <c r="W7" s="13"/>
       <c r="Y7" s="11"/>
@@ -1045,21 +1098,21 @@
       <c r="AJ7" s="11"/>
     </row>
     <row r="8">
-      <c r="A8" s="15"/>
+      <c r="A8" s="14"/>
       <c r="B8" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>31</v>
-      </c>
       <c r="D8" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>18</v>
+        <v>30</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
@@ -1073,7 +1126,8 @@
       <c r="P8" s="11"/>
       <c r="Q8" s="11"/>
       <c r="R8" s="11"/>
-      <c r="S8" s="13"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
       <c r="U8" s="13"/>
       <c r="W8" s="13"/>
       <c r="Y8" s="11"/>
@@ -1092,34 +1146,34 @@
     <row r="9">
       <c r="A9" s="15"/>
       <c r="B9" s="9" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>22</v>
+        <v>31</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
-      <c r="I9" s="10" t="s">
-        <v>18</v>
+      <c r="I9" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K9" s="11"/>
       <c r="L9" s="11"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
       <c r="S9" s="13"/>
       <c r="U9" s="13"/>
       <c r="W9" s="13"/>
@@ -1139,48 +1193,34 @@
     <row r="10">
       <c r="A10" s="15"/>
       <c r="B10" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>37</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C10" s="9"/>
       <c r="D10" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>22</v>
+        <v>33</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="J10" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="K10" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="L10" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="M10" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="N10" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
-      <c r="Q10" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="R10" s="10" t="s">
-        <v>43</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
       <c r="S10" s="13"/>
       <c r="U10" s="13"/>
       <c r="W10" s="13"/>
@@ -1200,26 +1240,26 @@
     <row r="11">
       <c r="A11" s="15"/>
       <c r="B11" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>22</v>
+      <c r="E11" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="J11" s="10" t="s">
-        <v>45</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
       <c r="K11" s="11"/>
       <c r="L11" s="11"/>
       <c r="M11" s="11"/>
@@ -1247,24 +1287,32 @@
     <row r="12">
       <c r="A12" s="15"/>
       <c r="B12" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="17"/>
+        <v>37</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="D12" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" s="13"/>
-      <c r="I12" s="11"/>
-      <c r="K12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="O12" s="13"/>
-      <c r="Q12" s="13"/>
+        <v>38</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
       <c r="S12" s="13"/>
       <c r="U12" s="13"/>
       <c r="W12" s="13"/>
@@ -1284,24 +1332,30 @@
     <row r="13">
       <c r="A13" s="15"/>
       <c r="B13" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="17"/>
+        <v>37</v>
+      </c>
+      <c r="C13" s="9"/>
       <c r="D13" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" s="13"/>
+        <v>38</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
       <c r="I13" s="12"/>
-      <c r="K13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="O13" s="13"/>
-      <c r="Q13" s="13"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
       <c r="S13" s="13"/>
       <c r="U13" s="13"/>
       <c r="W13" s="13"/>
@@ -1321,24 +1375,32 @@
     <row r="14">
       <c r="A14" s="15"/>
       <c r="B14" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="17"/>
+        <v>40</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>41</v>
+      </c>
       <c r="D14" s="9" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="G14" s="13"/>
+        <v>26</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
       <c r="I14" s="12"/>
-      <c r="K14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="O14" s="13"/>
-      <c r="Q14" s="13"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
       <c r="S14" s="13"/>
       <c r="U14" s="13"/>
       <c r="W14" s="13"/>
@@ -1358,24 +1420,32 @@
     <row r="15">
       <c r="A15" s="15"/>
       <c r="B15" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="17"/>
+        <v>40</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>41</v>
+      </c>
       <c r="D15" s="9" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="E15" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="G15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="O15" s="13"/>
-      <c r="Q15" s="13"/>
+      <c r="F15" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
       <c r="S15" s="13"/>
       <c r="U15" s="13"/>
       <c r="W15" s="13"/>
@@ -1395,24 +1465,36 @@
     <row r="16">
       <c r="A16" s="15"/>
       <c r="B16" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="17"/>
+        <v>40</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>41</v>
+      </c>
       <c r="D16" s="9" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="G16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="O16" s="13"/>
-      <c r="Q16" s="13"/>
+        <v>18</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
       <c r="S16" s="13"/>
       <c r="U16" s="13"/>
       <c r="W16" s="13"/>
@@ -1432,24 +1514,44 @@
     <row r="17">
       <c r="A17" s="15"/>
       <c r="B17" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="17"/>
+        <v>40</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>41</v>
+      </c>
       <c r="D17" s="9" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="K17" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="L17" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="M17" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N17" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="G17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="O17" s="13"/>
-      <c r="Q17" s="13"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
       <c r="S17" s="13"/>
       <c r="U17" s="13"/>
       <c r="W17" s="13"/>
@@ -1469,24 +1571,30 @@
     <row r="18">
       <c r="A18" s="15"/>
       <c r="B18" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="17"/>
+        <v>52</v>
+      </c>
+      <c r="C18" s="9"/>
       <c r="D18" s="9" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="G18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="O18" s="13"/>
-      <c r="Q18" s="13"/>
+        <v>26</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
       <c r="S18" s="13"/>
       <c r="U18" s="13"/>
       <c r="W18" s="13"/>
@@ -1506,24 +1614,34 @@
     <row r="19">
       <c r="A19" s="15"/>
       <c r="B19" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="17"/>
+        <v>54</v>
+      </c>
+      <c r="C19" s="9"/>
       <c r="D19" s="9" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F19" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="G19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="O19" s="13"/>
-      <c r="Q19" s="13"/>
+        <v>26</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
       <c r="S19" s="13"/>
       <c r="U19" s="13"/>
       <c r="W19" s="13"/>
@@ -1543,24 +1661,48 @@
     <row r="20">
       <c r="A20" s="15"/>
       <c r="B20" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="17"/>
+        <v>57</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>58</v>
+      </c>
       <c r="D20" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F20" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="G20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="Q20" s="13"/>
+        <v>58</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="K20" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="L20" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="M20" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="N20" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="R20" s="10" t="s">
+        <v>60</v>
+      </c>
       <c r="S20" s="13"/>
       <c r="U20" s="13"/>
       <c r="W20" s="13"/>
@@ -1580,24 +1722,34 @@
     <row r="21">
       <c r="A21" s="15"/>
       <c r="B21" s="9" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="C21" s="17"/>
       <c r="D21" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F21" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="G21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="Q21" s="13"/>
+        <v>58</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J21" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
       <c r="S21" s="13"/>
       <c r="U21" s="13"/>
       <c r="W21" s="13"/>
@@ -1617,20 +1769,20 @@
     <row r="22">
       <c r="A22" s="15"/>
       <c r="B22" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="17"/>
+        <v>57</v>
+      </c>
+      <c r="C22" s="18"/>
       <c r="D22" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F22" s="18" t="s">
-        <v>56</v>
+        <v>58</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>63</v>
       </c>
       <c r="G22" s="13"/>
-      <c r="I22" s="13"/>
+      <c r="I22" s="11"/>
       <c r="K22" s="13"/>
       <c r="M22" s="13"/>
       <c r="O22" s="13"/>
@@ -1654,20 +1806,20 @@
     <row r="23">
       <c r="A23" s="15"/>
       <c r="B23" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="17"/>
+        <v>57</v>
+      </c>
+      <c r="C23" s="18"/>
       <c r="D23" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F23" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>64</v>
       </c>
       <c r="G23" s="13"/>
-      <c r="I23" s="13"/>
+      <c r="I23" s="12"/>
       <c r="K23" s="13"/>
       <c r="M23" s="13"/>
       <c r="O23" s="13"/>
@@ -1691,20 +1843,20 @@
     <row r="24">
       <c r="A24" s="15"/>
       <c r="B24" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="17"/>
+        <v>57</v>
+      </c>
+      <c r="C24" s="18"/>
       <c r="D24" s="9" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F24" s="18" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>65</v>
       </c>
       <c r="G24" s="13"/>
-      <c r="I24" s="13"/>
+      <c r="I24" s="12"/>
       <c r="K24" s="13"/>
       <c r="M24" s="13"/>
       <c r="O24" s="13"/>
@@ -1728,17 +1880,17 @@
     <row r="25">
       <c r="A25" s="15"/>
       <c r="B25" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" s="17"/>
+        <v>57</v>
+      </c>
+      <c r="C25" s="18"/>
       <c r="D25" s="9" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F25" s="18" t="s">
-        <v>59</v>
+        <v>18</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>66</v>
       </c>
       <c r="G25" s="13"/>
       <c r="I25" s="13"/>
@@ -1765,25 +1917,20 @@
     <row r="26">
       <c r="A26" s="15"/>
       <c r="B26" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="17"/>
+        <v>57</v>
+      </c>
+      <c r="C26" s="18"/>
       <c r="D26" s="9" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F26" s="18" t="s">
-        <v>60</v>
+        <v>26</v>
+      </c>
+      <c r="F26" s="19" t="s">
+        <v>67</v>
       </c>
       <c r="G26" s="13"/>
-      <c r="I26" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="J26" s="18" t="s">
-        <v>62</v>
-      </c>
+      <c r="I26" s="13"/>
       <c r="K26" s="13"/>
       <c r="M26" s="13"/>
       <c r="O26" s="13"/>
@@ -1807,25 +1954,20 @@
     <row r="27">
       <c r="A27" s="15"/>
       <c r="B27" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" s="17"/>
+        <v>57</v>
+      </c>
+      <c r="C27" s="18"/>
       <c r="D27" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E27" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="F27" s="18" t="s">
-        <v>63</v>
+        <v>58</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F27" s="19" t="s">
+        <v>68</v>
       </c>
       <c r="G27" s="13"/>
-      <c r="I27" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="J27" s="18" t="s">
-        <v>60</v>
-      </c>
+      <c r="I27" s="13"/>
       <c r="K27" s="13"/>
       <c r="M27" s="13"/>
       <c r="O27" s="13"/>
@@ -1846,6 +1988,386 @@
       <c r="AI27" s="11"/>
       <c r="AJ27" s="11"/>
     </row>
+    <row r="28">
+      <c r="A28" s="15"/>
+      <c r="B28" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="18"/>
+      <c r="D28" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="G28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="O28" s="13"/>
+      <c r="Q28" s="13"/>
+      <c r="S28" s="13"/>
+      <c r="U28" s="13"/>
+      <c r="W28" s="13"/>
+      <c r="Y28" s="11"/>
+      <c r="Z28" s="11"/>
+      <c r="AA28" s="11"/>
+      <c r="AB28" s="11"/>
+      <c r="AC28" s="11"/>
+      <c r="AD28" s="11"/>
+      <c r="AE28" s="11"/>
+      <c r="AF28" s="11"/>
+      <c r="AG28" s="11"/>
+      <c r="AH28" s="11"/>
+      <c r="AI28" s="11"/>
+      <c r="AJ28" s="11"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="15"/>
+      <c r="B29" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="18"/>
+      <c r="D29" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F29" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="G29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="O29" s="13"/>
+      <c r="Q29" s="13"/>
+      <c r="S29" s="13"/>
+      <c r="U29" s="13"/>
+      <c r="W29" s="13"/>
+      <c r="Y29" s="11"/>
+      <c r="Z29" s="11"/>
+      <c r="AA29" s="11"/>
+      <c r="AB29" s="11"/>
+      <c r="AC29" s="11"/>
+      <c r="AD29" s="11"/>
+      <c r="AE29" s="11"/>
+      <c r="AF29" s="11"/>
+      <c r="AG29" s="11"/>
+      <c r="AH29" s="11"/>
+      <c r="AI29" s="11"/>
+      <c r="AJ29" s="11"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="15"/>
+      <c r="B30" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="18"/>
+      <c r="D30" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F30" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="G30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="O30" s="13"/>
+      <c r="Q30" s="13"/>
+      <c r="S30" s="13"/>
+      <c r="U30" s="13"/>
+      <c r="W30" s="13"/>
+      <c r="Y30" s="11"/>
+      <c r="Z30" s="11"/>
+      <c r="AA30" s="11"/>
+      <c r="AB30" s="11"/>
+      <c r="AC30" s="11"/>
+      <c r="AD30" s="11"/>
+      <c r="AE30" s="11"/>
+      <c r="AF30" s="11"/>
+      <c r="AG30" s="11"/>
+      <c r="AH30" s="11"/>
+      <c r="AI30" s="11"/>
+      <c r="AJ30" s="11"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="15"/>
+      <c r="B31" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="18"/>
+      <c r="D31" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F31" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="G31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="O31" s="13"/>
+      <c r="Q31" s="13"/>
+      <c r="S31" s="13"/>
+      <c r="U31" s="13"/>
+      <c r="W31" s="13"/>
+      <c r="Y31" s="11"/>
+      <c r="Z31" s="11"/>
+      <c r="AA31" s="11"/>
+      <c r="AB31" s="11"/>
+      <c r="AC31" s="11"/>
+      <c r="AD31" s="11"/>
+      <c r="AE31" s="11"/>
+      <c r="AF31" s="11"/>
+      <c r="AG31" s="11"/>
+      <c r="AH31" s="11"/>
+      <c r="AI31" s="11"/>
+      <c r="AJ31" s="11"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="15"/>
+      <c r="B32" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="18"/>
+      <c r="D32" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="G32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="Q32" s="13"/>
+      <c r="S32" s="13"/>
+      <c r="U32" s="13"/>
+      <c r="W32" s="13"/>
+      <c r="Y32" s="11"/>
+      <c r="Z32" s="11"/>
+      <c r="AA32" s="11"/>
+      <c r="AB32" s="11"/>
+      <c r="AC32" s="11"/>
+      <c r="AD32" s="11"/>
+      <c r="AE32" s="11"/>
+      <c r="AF32" s="11"/>
+      <c r="AG32" s="11"/>
+      <c r="AH32" s="11"/>
+      <c r="AI32" s="11"/>
+      <c r="AJ32" s="11"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="15"/>
+      <c r="B33" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="18"/>
+      <c r="D33" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F33" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="G33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="O33" s="13"/>
+      <c r="Q33" s="13"/>
+      <c r="S33" s="13"/>
+      <c r="U33" s="13"/>
+      <c r="W33" s="13"/>
+      <c r="Y33" s="11"/>
+      <c r="Z33" s="11"/>
+      <c r="AA33" s="11"/>
+      <c r="AB33" s="11"/>
+      <c r="AC33" s="11"/>
+      <c r="AD33" s="11"/>
+      <c r="AE33" s="11"/>
+      <c r="AF33" s="11"/>
+      <c r="AG33" s="11"/>
+      <c r="AH33" s="11"/>
+      <c r="AI33" s="11"/>
+      <c r="AJ33" s="11"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="15"/>
+      <c r="B34" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="18"/>
+      <c r="D34" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F34" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="G34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="M34" s="13"/>
+      <c r="O34" s="13"/>
+      <c r="Q34" s="13"/>
+      <c r="S34" s="13"/>
+      <c r="U34" s="13"/>
+      <c r="W34" s="13"/>
+      <c r="Y34" s="11"/>
+      <c r="Z34" s="11"/>
+      <c r="AA34" s="11"/>
+      <c r="AB34" s="11"/>
+      <c r="AC34" s="11"/>
+      <c r="AD34" s="11"/>
+      <c r="AE34" s="11"/>
+      <c r="AF34" s="11"/>
+      <c r="AG34" s="11"/>
+      <c r="AH34" s="11"/>
+      <c r="AI34" s="11"/>
+      <c r="AJ34" s="11"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="15"/>
+      <c r="B35" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C35" s="18"/>
+      <c r="D35" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F35" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="G35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="K35" s="13"/>
+      <c r="M35" s="13"/>
+      <c r="O35" s="13"/>
+      <c r="Q35" s="13"/>
+      <c r="S35" s="13"/>
+      <c r="U35" s="13"/>
+      <c r="W35" s="13"/>
+      <c r="Y35" s="11"/>
+      <c r="Z35" s="11"/>
+      <c r="AA35" s="11"/>
+      <c r="AB35" s="11"/>
+      <c r="AC35" s="11"/>
+      <c r="AD35" s="11"/>
+      <c r="AE35" s="11"/>
+      <c r="AF35" s="11"/>
+      <c r="AG35" s="11"/>
+      <c r="AH35" s="11"/>
+      <c r="AI35" s="11"/>
+      <c r="AJ35" s="11"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="15"/>
+      <c r="B36" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="18"/>
+      <c r="D36" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F36" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="G36" s="13"/>
+      <c r="I36" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="J36" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="K36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="O36" s="13"/>
+      <c r="Q36" s="13"/>
+      <c r="S36" s="13"/>
+      <c r="U36" s="13"/>
+      <c r="W36" s="13"/>
+      <c r="Y36" s="11"/>
+      <c r="Z36" s="11"/>
+      <c r="AA36" s="11"/>
+      <c r="AB36" s="11"/>
+      <c r="AC36" s="11"/>
+      <c r="AD36" s="11"/>
+      <c r="AE36" s="11"/>
+      <c r="AF36" s="11"/>
+      <c r="AG36" s="11"/>
+      <c r="AH36" s="11"/>
+      <c r="AI36" s="11"/>
+      <c r="AJ36" s="11"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="15"/>
+      <c r="B37" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" s="18"/>
+      <c r="D37" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E37" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="F37" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G37" s="13"/>
+      <c r="I37" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J37" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="K37" s="13"/>
+      <c r="M37" s="13"/>
+      <c r="O37" s="13"/>
+      <c r="Q37" s="13"/>
+      <c r="S37" s="13"/>
+      <c r="U37" s="13"/>
+      <c r="W37" s="13"/>
+      <c r="Y37" s="11"/>
+      <c r="Z37" s="11"/>
+      <c r="AA37" s="11"/>
+      <c r="AB37" s="11"/>
+      <c r="AC37" s="11"/>
+      <c r="AD37" s="11"/>
+      <c r="AE37" s="11"/>
+      <c r="AF37" s="11"/>
+      <c r="AG37" s="11"/>
+      <c r="AH37" s="11"/>
+      <c r="AI37" s="11"/>
+      <c r="AJ37" s="11"/>
+    </row>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="Q1:T1"/>
@@ -1862,7 +2384,7 @@
     <mergeCell ref="M1:P1"/>
   </mergeCells>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3:E27 G3:G27 I3:I27 K3:K27 M3:M27 O3:O27 Q3:Q27 S3:S27 U3:U27 W3:W27 Y3:Y27 AA3:AA27 AC3:AC27 AE3:AE27 AG3:AG27 AI3:AI27">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3:E37 G3:G37 I3:I37 K3:K37 M3:M37 O3:O37 Q3:Q37 S3:S37 U3:U37 W3:W37 Y3:Y37 AA3:AA37 AC3:AC37 AE3:AE37 AG3:AG37 AI3:AI37">
       <formula1>'Rule types'!$A$3:$A$100</formula1>
     </dataValidation>
   </dataValidations>
@@ -1881,148 +2403,148 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="19" t="s">
-        <v>64</v>
+      <c r="A1" s="20" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="18" t="s">
-        <v>38</v>
+      <c r="A3" s="19" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="18" t="s">
-        <v>65</v>
+      <c r="A4" s="19" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="18" t="s">
-        <v>66</v>
+      <c r="A5" s="19" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="18" t="s">
-        <v>22</v>
+      <c r="A6" s="19" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="18" t="s">
-        <v>67</v>
+      <c r="A7" s="19" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="18" t="s">
-        <v>68</v>
+      <c r="A8" s="19" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="18" t="s">
-        <v>69</v>
+      <c r="A9" s="19" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="18" t="s">
-        <v>70</v>
+      <c r="A10" s="19" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="18" t="s">
-        <v>71</v>
+      <c r="A11" s="19" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="18" t="s">
-        <v>72</v>
+      <c r="A12" s="19" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="18" t="s">
-        <v>73</v>
+      <c r="A13" s="19" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="18" t="s">
-        <v>74</v>
+      <c r="A14" s="19" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="18" t="s">
-        <v>75</v>
+      <c r="A15" s="19" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="18" t="s">
-        <v>76</v>
+      <c r="A16" s="19" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="18" t="s">
-        <v>77</v>
+      <c r="A17" s="19" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="19" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="19" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="18" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="18" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="18" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="18" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="18" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="18" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="18" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="18" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="18" t="s">
-        <v>61</v>
-      </c>
-    </row>
     <row r="29">
-      <c r="A29" s="18" t="s">
-        <v>40</v>
+      <c r="A29" s="19" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="18" t="s">
-        <v>87</v>
+      <c r="A30" s="19" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2047,8 +2569,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="20" t="s">
-        <v>88</v>
+      <c r="A1" s="21" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>